<commit_message>
interfaces second last change today
</commit_message>
<xml_diff>
--- a/Emad Branch/inertfaces.xlsx
+++ b/Emad Branch/inertfaces.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="843" firstSheet="10" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="843" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="2" r:id="rId1"/>
@@ -26,8 +26,9 @@
     <sheet name="إعارة كتاب" sheetId="5" r:id="rId12"/>
     <sheet name="حذف كتاب" sheetId="17" r:id="rId13"/>
     <sheet name="الإستعلام عن الكتاب" sheetId="6" r:id="rId14"/>
-    <sheet name="الإستعلام عن المحذوفة" sheetId="23" r:id="rId15"/>
-    <sheet name="الإستعلام عن الغرامات" sheetId="39" r:id="rId16"/>
+    <sheet name="الإستعلام عن الكتب المستعارة" sheetId="40" r:id="rId15"/>
+    <sheet name="الإستعلام عن الكتب المحذوفة" sheetId="23" r:id="rId16"/>
+    <sheet name="الإستعلام عن الغرامات" sheetId="39" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="82">
   <si>
     <t>أسم الموظف</t>
   </si>
@@ -282,6 +283,9 @@
   </si>
   <si>
     <t>طباعة</t>
+  </si>
+  <si>
+    <t>الإستعلام عن الكتب المستعارة</t>
   </si>
 </sst>
 </file>
@@ -754,6 +758,23 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -765,16 +786,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -789,9 +814,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -801,19 +823,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -822,11 +831,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1356,12 +1360,12 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:5" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="2:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
@@ -1391,15 +1395,15 @@
     </row>
     <row r="7" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="20" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1430,26 +1434,26 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="2:5" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="12" t="s">
         <v>66</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-      <c r="C5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="12" t="s">
         <v>69</v>
       </c>
@@ -1477,22 +1481,22 @@
     </row>
     <row r="8" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="20" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1512,7 +1516,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D4" activeCellId="1" sqref="B4:B6 D4:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1525,12 +1529,12 @@
   <sheetData>
     <row r="2" spans="2:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
@@ -1564,22 +1568,22 @@
     </row>
     <row r="7" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="19" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="20" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1608,27 +1612,27 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:4" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="2:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
     </row>
     <row r="6" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="21" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1646,7 +1650,7 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="B2:D19"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView rightToLeft="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -1659,11 +1663,11 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:4" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1675,23 +1679,23 @@
     </row>
     <row r="6" spans="2:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="21" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="41"/>
+      <c r="B9" s="18"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D10" s="41"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
+      <c r="B11" s="18"/>
       <c r="D11" t="s">
         <v>76</v>
       </c>
@@ -1708,39 +1712,39 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
     </row>
     <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1753,6 +1757,131 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G14"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="15.75" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
+    <col min="9" max="9" width="14.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="2:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="2:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="B2:E14"/>
@@ -1771,12 +1900,12 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="2:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
@@ -1793,55 +1922,55 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="2:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="21" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="20" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1853,13 +1982,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1871,14 +2000,14 @@
   <sheetData>
     <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
@@ -1901,69 +2030,69 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="2:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="21" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="44" t="s">
+      <c r="G14" s="20" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1993,35 +2122,35 @@
   <sheetData>
     <row r="2" spans="2:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="2:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
     </row>
     <row r="5" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
     </row>
     <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="41"/>
-      <c r="D8" s="42" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="41"/>
+      <c r="B9" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2052,53 +2181,53 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="23"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
     </row>
     <row r="5" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="24"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="2:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="24"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="24"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="2:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="25"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
     </row>
     <row r="9" spans="2:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="25"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
     </row>
     <row r="10" spans="2:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
@@ -2134,29 +2263,29 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="27"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
     </row>
     <row r="4" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="23"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
     </row>
     <row r="5" spans="2:4" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="20" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2189,14 +2318,14 @@
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
@@ -2256,19 +2385,19 @@
     </row>
     <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="44" t="s">
+      <c r="G14" s="20" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2300,14 +2429,14 @@
   <sheetData>
     <row r="2" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="3:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="12" t="s">
@@ -2331,9 +2460,9 @@
       <c r="E5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="3:8" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="12" t="s">
@@ -2343,37 +2472,37 @@
       <c r="E6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="45"/>
     </row>
     <row r="7" spans="3:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="22"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="9" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="3:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="3:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H13" s="44" t="s">
+      <c r="H13" s="20" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2406,25 +2535,25 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="27"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
     </row>
     <row r="4" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="23"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
     </row>
     <row r="5" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="24"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
@@ -2464,16 +2593,16 @@
   <sheetData>
     <row r="2" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:8" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="3:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="12" t="s">
@@ -2514,27 +2643,27 @@
         <v>24</v>
       </c>
       <c r="D7" s="13"/>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="39"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="3:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="3:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="3:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="3:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H12" s="44" t="s">
+      <c r="H12" s="20" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2566,14 +2695,14 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="2:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
@@ -2586,112 +2715,113 @@
       <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="32"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="22"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="45"/>
     </row>
     <row r="8" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="45"/>
     </row>
     <row r="11" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="34"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
     </row>
     <row r="12" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="45"/>
     </row>
     <row r="13" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="45"/>
     </row>
     <row r="14" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="45"/>
     </row>
     <row r="15" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="22"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="32"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="22"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="32"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="22"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="32"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="22"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="32"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="22"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="22"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="29"/>
     </row>
     <row r="22" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="20" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B15:E15"/>
@@ -2708,7 +2838,6 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>